<commit_message>
passes ilie and My tests
</commit_message>
<xml_diff>
--- a/data/tests/traceTest.xlsx
+++ b/data/tests/traceTest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1628465_ed_ac_uk/Documents/Year5/PA/CW2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James H\git\CacheSimulator\data\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="11_F25DC773A252ABDACC10489891195DEA5BDE58E6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{72DEBD05-F886-4D65-BD35-3C03BBC904DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF712994-1515-4577-9A59-9219A0CFFD75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,13 +651,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C4" s="1">
         <v>1</v>
       </c>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C5" s="1">
         <v>2</v>
       </c>
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C6" s="1">
         <v>3</v>
       </c>
@@ -822,7 +822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>4</v>
       </c>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <v>5</v>
       </c>
@@ -905,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <v>6</v>
       </c>
@@ -946,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <v>7</v>
       </c>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
         <v>8</v>
       </c>
@@ -1020,16 +1020,16 @@
         <v>0</v>
       </c>
       <c r="M11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
         <v>9</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
@@ -1107,12 +1107,12 @@
         <v>1</v>
       </c>
       <c r="M13" s="19">
-        <f t="shared" ref="K13:O13" si="0">SUM(M4:M12)</f>
-        <v>1</v>
+        <f t="shared" ref="M13:O13" si="0">SUM(M4:M12)</f>
+        <v>0</v>
       </c>
       <c r="N13" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="20">
         <f t="shared" si="0"/>

</xml_diff>